<commit_message>
fixing uploading large files
</commit_message>
<xml_diff>
--- a/public/uploads/stocks/stock_list_3.xlsx
+++ b/public/uploads/stocks/stock_list_3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -580,7 +580,7 @@
   <dimension ref="A1:N521"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -665,7 +665,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1">
-        <v>445566</v>
+        <v>321</v>
       </c>
       <c r="I2" s="4">
         <v>42880</v>
@@ -710,7 +710,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="1">
-        <v>32456</v>
+        <v>322</v>
       </c>
       <c r="I3" s="4">
         <v>44114</v>
@@ -755,7 +755,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="6">
-        <v>12345</v>
+        <v>323</v>
       </c>
       <c r="I4" s="7">
         <v>41255</v>

</xml_diff>